<commit_message>
updated caml project with report
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11340" windowHeight="1935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10545" windowHeight="3030"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -28,16 +27,13 @@
     <t>Password</t>
   </si>
   <si>
+    <t>s6670405</t>
+  </si>
+  <si>
     <t>TEST123</t>
   </si>
   <si>
-    <t>s6670405</t>
-  </si>
-  <si>
-    <t>a5417458</t>
-  </si>
-  <si>
-    <t>Test24501</t>
+    <t>Quality77</t>
   </si>
 </sst>
 </file>
@@ -388,18 +384,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>